<commit_message>
1 Day 1 Commit
</commit_message>
<xml_diff>
--- a/Code-specific differences.xlsx
+++ b/Code-specific differences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\Codecademy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B91C61-BC46-472E-9D81-8D03D5583C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C07EFC-6217-4AD4-885D-1ED30774540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="210" windowWidth="21600" windowHeight="13950" xr2:uid="{A31A3DCD-58E5-4D02-8B31-6FF2806C58F6}"/>
+    <workbookView xWindow="-28395" yWindow="8385" windowWidth="18900" windowHeight="14880" xr2:uid="{A31A3DCD-58E5-4D02-8B31-6FF2806C58F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>C+</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,6 +85,38 @@
   </si>
   <si>
     <t>Print("Hallo")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>printf("")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scanf("")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조건문
+conditional</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반복문
+loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if
+switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>while (condition) { // Statement(s) }
+do {  // Statement(s) } while (condition);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -92,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +143,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -197,7 +237,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -227,6 +267,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,18 +591,19 @@
   <dimension ref="C4:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.625" customWidth="1"/>
+    <col min="1" max="1" width="4.58203125" customWidth="1"/>
     <col min="2" max="2" width="3.5" customWidth="1"/>
-    <col min="3" max="3" width="13.125" style="1" customWidth="1"/>
-    <col min="4" max="10" width="18.125" customWidth="1"/>
+    <col min="3" max="3" width="13.08203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.75" customWidth="1"/>
+    <col min="5" max="10" width="18.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
         <v>1</v>
@@ -580,7 +627,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="34" x14ac:dyDescent="0.45">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
@@ -598,11 +645,13 @@
       </c>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -614,9 +663,13 @@
       </c>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="3"/>
-      <c r="D7" s="7"/>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.45">
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -624,9 +677,13 @@
       <c r="I7" s="8"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
+    <row r="8" spans="3:10" ht="34" x14ac:dyDescent="0.45">
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -634,9 +691,13 @@
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
+    <row r="9" spans="3:10" ht="34.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -644,7 +705,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C10" s="3"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -654,7 +715,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C11" s="3"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -664,7 +725,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C12" s="3"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -674,7 +735,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C13" s="3"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -684,7 +745,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C14" s="3"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -694,7 +755,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C15" s="3"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -704,7 +765,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C16" s="3"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -714,7 +775,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C17" s="3"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -724,7 +785,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C18" s="3"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -734,7 +795,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C19" s="3"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -744,7 +805,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C20" s="3"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -754,7 +815,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C21" s="3"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -764,7 +825,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C22" s="3"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -774,7 +835,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C23" s="3"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -784,7 +845,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C24" s="3"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -794,7 +855,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C25" s="3"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -804,7 +865,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C26" s="3"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -814,7 +875,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" x14ac:dyDescent="0.45">
       <c r="C27" s="3"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>

</xml_diff>